<commit_message>
YTI-1103: Datamodel changes according to design regarding members and their membervalues. Bugfixes.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634DF80C-CBE4-684C-BACE-ED6EA5F46ABC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3BFCE-A296-4841-9E5C-6146E83C9A21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" activeTab="3" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" activeTab="4" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -634,18 +634,12 @@
     <t>calculationHierarchy</t>
   </si>
   <si>
-    <t>MEMBERVALUE_1</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
     <t>=</t>
   </si>
   <si>
-    <t>MEMBERVALUE_2</t>
-  </si>
-  <si>
     <t>Laajennus 3 suomeksi</t>
   </si>
   <si>
@@ -782,6 +776,12 @@
   </si>
   <si>
     <t>Laajennus 25 suomeksi</t>
+  </si>
+  <si>
+    <t>UNARYOPERATOR</t>
+  </si>
+  <si>
+    <t>COMPARISONOPERATOR</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F821AE-14EF-9447-94FD-816F31696438}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -2289,10 +2289,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -2306,10 +2306,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -2323,10 +2323,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -2340,10 +2340,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -2357,10 +2357,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -2374,10 +2374,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
@@ -2391,10 +2391,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
@@ -2408,10 +2408,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
         <v>72</v>
@@ -2425,10 +2425,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D12" t="s">
         <v>76</v>
@@ -2442,10 +2442,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D13" t="s">
         <v>78</v>
@@ -2459,10 +2459,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
@@ -2473,10 +2473,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>109</v>
@@ -2487,10 +2487,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D16" t="s">
         <v>110</v>
@@ -2501,10 +2501,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>189</v>
@@ -2515,10 +2515,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D18" t="s">
         <v>111</v>
@@ -2529,10 +2529,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D19" t="s">
         <v>112</v>
@@ -2543,10 +2543,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D20" t="s">
         <v>113</v>
@@ -2557,10 +2557,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D21" t="s">
         <v>114</v>
@@ -2571,10 +2571,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>119</v>
@@ -2585,10 +2585,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D23" t="s">
         <v>115</v>
@@ -2599,10 +2599,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D24" t="s">
         <v>116</v>
@@ -2613,10 +2613,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D25" t="s">
         <v>117</v>
@@ -2627,10 +2627,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D26" t="s">
         <v>118</v>
@@ -2645,8 +2645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABC4F1-E3E2-CE4D-BF77-D99DAF76AC27}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2662,10 +2662,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="C1" t="s">
         <v>94</v>
@@ -2685,10 +2685,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" t="s">
         <v>202</v>
-      </c>
-      <c r="B2" t="s">
-        <v>203</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
         <v>202</v>
-      </c>
-      <c r="B3" t="s">
-        <v>203</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2728,19 +2728,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
         <v>202</v>
-      </c>
-      <c r="B4" t="s">
-        <v>203</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -2751,19 +2751,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
         <v>202</v>
-      </c>
-      <c r="B5" t="s">
-        <v>203</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -2774,19 +2774,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" t="s">
         <v>202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -2797,19 +2797,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
         <v>202</v>
       </c>
-      <c r="B7" t="s">
-        <v>203</v>
-      </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -2820,19 +2820,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
         <v>202</v>
-      </c>
-      <c r="B8" t="s">
-        <v>203</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
@@ -2843,19 +2843,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" t="s">
         <v>202</v>
-      </c>
-      <c r="B9" t="s">
-        <v>203</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -2866,19 +2866,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" t="s">
         <v>202</v>
-      </c>
-      <c r="B10" t="s">
-        <v>203</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
@@ -2889,19 +2889,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" t="s">
         <v>202</v>
-      </c>
-      <c r="B11" t="s">
-        <v>203</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Fixing integration tests to better verify data imports.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3BFCE-A296-4841-9E5C-6146E83C9A21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70003FF-FB7C-8142-92D2-4B173D5C8867}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" activeTab="4" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -358,39 +358,6 @@
     <t>http://uri.suomi.fi/codelist/eu/dcat</t>
   </si>
   <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/AGRI</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/ECON</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/ENER</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/HEAL</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/INTR</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/JUST</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/REGI</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/SOCI</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/TECH</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/TRAN</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/GOVE</t>
-  </si>
-  <si>
     <t>LEGALBASE</t>
   </si>
   <si>
@@ -598,9 +565,6 @@
     <t>http://uri.suomi.fi/terminology/kira/KILIID111</t>
   </si>
   <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat/EDUC</t>
-  </si>
-  <si>
     <t>Laajennus 1 suomeksi</t>
   </si>
   <si>
@@ -782,6 +746,42 @@
   </si>
   <si>
     <t>COMPARISONOPERATOR</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/AGRI</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/ECON</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/EDUC</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/ENER</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/HEAL</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/INTR</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/JUST</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/GOVE</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/REGI</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/SOCI</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/TECH</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat/code/TRAN</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -1194,13 +1194,13 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -1209,25 +1209,25 @@
         <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="N1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="O1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="P1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="Q1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="R1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="S1" t="s">
         <v>13</v>
@@ -1253,19 +1253,19 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="H2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -1277,25 +1277,25 @@
         <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="N2" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="O2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="P2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="Q2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>19</v>
@@ -1307,7 +1307,7 @@
         <v>97</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1353,13 +1353,13 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
@@ -1385,13 +1385,13 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
@@ -1417,10 +1417,10 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -1446,10 +1446,10 @@
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>19</v>
@@ -1475,10 +1475,10 @@
         <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>19</v>
@@ -1504,10 +1504,10 @@
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>19</v>
@@ -1533,10 +1533,10 @@
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>19</v>
@@ -1562,10 +1562,10 @@
         <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -1591,10 +1591,10 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G9" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>19</v>
@@ -1620,10 +1620,10 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>19</v>
@@ -1649,10 +1649,10 @@
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>19</v>
@@ -1678,10 +1678,10 @@
         <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G12" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>19</v>
@@ -1707,10 +1707,10 @@
         <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>19</v>
@@ -1736,10 +1736,10 @@
         <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G14" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>19</v>
@@ -1765,10 +1765,10 @@
         <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>19</v>
@@ -1794,10 +1794,10 @@
         <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>19</v>
@@ -1823,10 +1823,10 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G17" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>19</v>
@@ -1852,10 +1852,10 @@
         <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>19</v>
@@ -1881,10 +1881,10 @@
         <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G19" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>19</v>
@@ -1910,10 +1910,10 @@
         <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="G20" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>19</v>
@@ -1939,10 +1939,10 @@
         <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G21" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>19</v>
@@ -1968,10 +1968,10 @@
         <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>19</v>
@@ -1997,10 +1997,10 @@
         <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G23" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>19</v>
@@ -2026,10 +2026,10 @@
         <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G24" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>19</v>
@@ -2055,10 +2055,10 @@
         <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="G25" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>19</v>
@@ -2084,10 +2084,10 @@
         <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="G26" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>19</v>
@@ -2109,7 +2109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2149,7 +2149,7 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2159,7 +2159,7 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D2" t="s">
@@ -2178,7 +2178,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2195,7 +2195,7 @@
         <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>19</v>
@@ -2204,13 +2204,10 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{75695AA1-87BD-844E-A47F-D8271C59B1D7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2221,16 +2218,15 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -2255,16 +2251,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2272,16 +2268,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
-        <v>110</v>
+      <c r="E3" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2289,16 +2285,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2306,16 +2302,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>111</v>
+      <c r="E5" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2323,16 +2319,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
-        <v>112</v>
+      <c r="E6" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2340,16 +2336,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
-        <v>113</v>
+      <c r="E7" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2357,16 +2353,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
-        <v>114</v>
+      <c r="E8" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2374,16 +2370,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>119</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2391,16 +2387,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" t="s">
-        <v>115</v>
+      <c r="E10" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2408,16 +2404,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
-        <v>116</v>
+      <c r="E11" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2425,16 +2421,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="E12" t="s">
-        <v>117</v>
+      <c r="E12" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2442,16 +2438,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
         <v>78</v>
       </c>
-      <c r="E13" t="s">
-        <v>118</v>
+      <c r="E13" s="3" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2459,10 +2455,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
@@ -2473,13 +2469,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2487,13 +2483,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
+        <v>225</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2501,13 +2497,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2515,13 +2511,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" t="s">
-        <v>111</v>
+        <v>227</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2529,13 +2525,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" t="s">
-        <v>112</v>
+        <v>228</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2543,13 +2539,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
-        <v>241</v>
-      </c>
-      <c r="D20" t="s">
-        <v>113</v>
+        <v>229</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2557,13 +2553,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C21" t="s">
-        <v>242</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
+        <v>230</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2571,13 +2567,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>119</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2585,13 +2581,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C23" t="s">
-        <v>244</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
+        <v>232</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2599,13 +2595,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C24" t="s">
-        <v>245</v>
-      </c>
-      <c r="D24" t="s">
-        <v>116</v>
+        <v>233</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2613,13 +2609,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C25" t="s">
-        <v>246</v>
-      </c>
-      <c r="D25" t="s">
-        <v>117</v>
+        <v>234</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2627,13 +2623,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C26" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
+        <v>235</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2645,7 +2641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABC4F1-E3E2-CE4D-BF77-D99DAF76AC27}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2662,10 +2658,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C1" t="s">
         <v>94</v>
@@ -2685,19 +2681,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -2705,19 +2701,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -2728,19 +2724,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -2751,19 +2747,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -2774,19 +2770,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -2797,19 +2793,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>201</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>202</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" t="s">
-        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -2820,19 +2816,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
@@ -2843,19 +2839,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -2866,19 +2862,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
@@ -2889,19 +2885,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F11" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Updating integration test Excel-files to use INFODOMAIN-header.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70003FF-FB7C-8142-92D2-4B173D5C8867}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E60A25-585D-C341-B8B1-895020CBB3BE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" activeTab="2" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Test code 01</t>
   </si>
   <si>
-    <t>CLASSIFICATION</t>
-  </si>
-  <si>
     <t>P9</t>
   </si>
   <si>
@@ -782,6 +779,9 @@
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/eu/dcat/code/TRAN</t>
+  </si>
+  <si>
+    <t>INFODOMAIN</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,25 +1182,25 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>250</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -1209,105 +1209,105 @@
         <v>2</v>
       </c>
       <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
         <v>110</v>
       </c>
-      <c r="M1" t="s">
-        <v>111</v>
-      </c>
       <c r="N1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" t="s">
         <v>175</v>
       </c>
-      <c r="P1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>115</v>
-      </c>
-      <c r="R1" t="s">
-        <v>176</v>
-      </c>
       <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
       <c r="U1" t="s">
+        <v>94</v>
+      </c>
+      <c r="V1" t="s">
         <v>95</v>
-      </c>
-      <c r="V1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
         <v>119</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>120</v>
-      </c>
-      <c r="H2" t="s">
-        <v>121</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
         <v>99</v>
       </c>
-      <c r="K2" t="s">
-        <v>100</v>
-      </c>
       <c r="L2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" t="s">
         <v>112</v>
       </c>
-      <c r="M2" t="s">
-        <v>113</v>
-      </c>
       <c r="N2" t="s">
+        <v>172</v>
+      </c>
+      <c r="O2" t="s">
         <v>173</v>
       </c>
-      <c r="O2" t="s">
-        <v>174</v>
-      </c>
       <c r="P2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" t="s">
         <v>116</v>
       </c>
-      <c r="Q2" t="s">
-        <v>117</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1353,19 +1353,19 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
       <c r="H1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1385,24 +1385,24 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1411,27 +1411,27 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1440,27 +1440,27 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1469,27 +1469,27 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1498,27 +1498,27 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1527,27 +1527,27 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1556,27 +1556,27 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1585,27 +1585,27 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1614,27 +1614,27 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1643,27 +1643,27 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1672,27 +1672,27 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1701,27 +1701,27 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
       <c r="F13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1730,27 +1730,27 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
       <c r="F14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1759,27 +1759,27 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
       <c r="F15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1788,27 +1788,27 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
       <c r="F16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1817,27 +1817,27 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1846,27 +1846,27 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1875,27 +1875,27 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
         <v>70</v>
       </c>
-      <c r="E19" t="s">
-        <v>71</v>
-      </c>
       <c r="F19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1904,27 +1904,27 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="E20" t="s">
-        <v>74</v>
-      </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -1933,27 +1933,27 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
         <v>81</v>
       </c>
-      <c r="E21" t="s">
-        <v>82</v>
-      </c>
       <c r="F21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1962,27 +1962,27 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
         <v>83</v>
       </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -1991,27 +1991,27 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
         <v>85</v>
       </c>
-      <c r="E23" t="s">
-        <v>86</v>
-      </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -2020,27 +2020,27 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
         <v>87</v>
       </c>
-      <c r="E24" t="s">
-        <v>88</v>
-      </c>
       <c r="F24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2049,27 +2049,27 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
         <v>89</v>
       </c>
-      <c r="E25" t="s">
-        <v>90</v>
-      </c>
       <c r="F25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2078,22 +2078,22 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
         <v>91</v>
       </c>
-      <c r="E26" t="s">
-        <v>92</v>
-      </c>
       <c r="F26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2109,7 +2109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4460C0-3790-E444-9C90-6BF5633E17FB}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2131,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2143,68 +2143,68 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2231,7 +2231,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2240,10 +2240,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2251,16 +2251,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>179</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2268,16 +2268,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
         <v>180</v>
       </c>
-      <c r="C3" t="s">
-        <v>181</v>
-      </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2285,16 +2285,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2302,16 +2302,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2319,16 +2319,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2336,16 +2336,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
         <v>201</v>
       </c>
-      <c r="C7" t="s">
-        <v>202</v>
-      </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2353,16 +2353,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2370,16 +2370,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2387,16 +2387,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2404,16 +2404,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2421,16 +2421,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2438,16 +2438,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2455,13 +2455,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2469,13 +2469,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2483,13 +2483,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2497,13 +2497,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2511,13 +2511,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2525,13 +2525,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2539,13 +2539,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2553,13 +2553,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2567,13 +2567,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2581,13 +2581,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2595,13 +2595,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2609,13 +2609,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2623,13 +2623,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2658,13 +2658,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
         <v>237</v>
       </c>
-      <c r="B1" t="s">
-        <v>238</v>
-      </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2673,27 +2673,27 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>189</v>
-      </c>
-      <c r="B2" t="s">
-        <v>190</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" t="s">
         <v>178</v>
-      </c>
-      <c r="E2" t="s">
-        <v>179</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -2701,22 +2701,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
         <v>189</v>
-      </c>
-      <c r="B3" t="s">
-        <v>190</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s">
         <v>180</v>
       </c>
-      <c r="E3" t="s">
-        <v>181</v>
-      </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -2724,186 +2724,186 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
         <v>189</v>
-      </c>
-      <c r="B4" t="s">
-        <v>190</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
         <v>189</v>
-      </c>
-      <c r="B5" t="s">
-        <v>190</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="s">
         <v>189</v>
-      </c>
-      <c r="B6" t="s">
-        <v>190</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
         <v>189</v>
       </c>
-      <c r="B7" t="s">
-        <v>190</v>
-      </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
         <v>201</v>
       </c>
-      <c r="E7" t="s">
-        <v>202</v>
-      </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" t="s">
-        <v>190</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" t="s">
         <v>189</v>
-      </c>
-      <c r="B9" t="s">
-        <v>190</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
         <v>189</v>
-      </c>
-      <c r="B10" t="s">
-        <v>190</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
         <v>189</v>
-      </c>
-      <c r="B11" t="s">
-        <v>190</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating integration test Excel-files to use INFORMATIONDOMAIN-header.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E60A25-585D-C341-B8B1-895020CBB3BE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B890AA0-3C41-AB45-AE94-62C46EBD788C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="31540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="8000" yWindow="460" windowWidth="25600" windowHeight="20540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
     <t>http://uri.suomi.fi/codelist/eu/dcat/code/TRAN</t>
   </si>
   <si>
-    <t>INFODOMAIN</t>
+    <t>INFORMATIONDOMAIN</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
YTI-879 - getting rid of the term classification. Intermediate commit.
Fixing Excel headers.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuukka\git\yti-codelist-content-intake-service\src\test\resources\codeschemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B890AA0-3C41-AB45-AE94-62C46EBD788C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058F345-04F1-46C2-A622-730185440631}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="460" windowWidth="25600" windowHeight="20540" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="7995" yWindow="465" windowWidth="25605" windowHeight="20535" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -1149,32 +1149,32 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="5" max="6" width="7.625" customWidth="1"/>
+    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.875" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" customWidth="1"/>
-    <col min="17" max="17" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.33203125" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.875" customWidth="1"/>
+    <col min="13" max="13" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.875" customWidth="1"/>
+    <col min="15" max="15" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.875" customWidth="1"/>
+    <col min="17" max="17" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.375" customWidth="1"/>
+    <col min="21" max="21" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1327,16 +1327,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2113,17 +2113,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2221,15 +2221,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2645,18 +2645,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>236</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>188</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>188</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>188</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>188</v>
       </c>

</xml_diff>

<commit_message>
YTI-696: Correcting integration test data according to new implementation.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
+++ b/src/test/resources/codeschemes/v1_codescheme_with_extensions_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuukka\git\yti-codelist-content-intake-service\src\test\resources\codeschemes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058F345-04F1-46C2-A622-730185440631}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFB9B9A-FC19-6041-8654-4B1633EB27DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="465" windowWidth="25605" windowHeight="20535" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" activeTab="4" xr2:uid="{A94C87D2-409E-C744-9409-8EB1E53C2CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Members_test_1" sheetId="4" r:id="rId4"/>
     <sheet name="Members_test_2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="260">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -782,6 +782,33 @@
   </si>
   <si>
     <t>INFORMATIONDOMAIN</t>
+  </si>
+  <si>
+    <t>code:testcode01</t>
+  </si>
+  <si>
+    <t>code:testcode03</t>
+  </si>
+  <si>
+    <t>code:testcode05</t>
+  </si>
+  <si>
+    <t>code:testcode07</t>
+  </si>
+  <si>
+    <t>code:testcode02</t>
+  </si>
+  <si>
+    <t>code:testcode04</t>
+  </si>
+  <si>
+    <t>code:testcode06</t>
+  </si>
+  <si>
+    <t>code:testcode08</t>
+  </si>
+  <si>
+    <t>code:testcode09</t>
   </si>
 </sst>
 </file>
@@ -1148,33 +1175,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3255037-6CC6-5342-A480-CDB6C5B76D51}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="6" width="7.625" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.875" customWidth="1"/>
+    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.875" customWidth="1"/>
-    <col min="13" max="13" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.875" customWidth="1"/>
-    <col min="15" max="15" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.875" customWidth="1"/>
-    <col min="17" max="17" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.375" customWidth="1"/>
-    <col min="21" max="21" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="17" max="17" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.33203125" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1269,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1327,16 +1354,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1400,7 +1427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1429,7 +1456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1458,7 +1485,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1487,7 +1514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1516,7 +1543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1545,7 +1572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1603,7 +1630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1632,7 +1659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1661,7 +1688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1690,7 +1717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1719,7 +1746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1748,7 +1775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1777,7 +1804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1806,7 +1833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1835,7 +1862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1864,7 +1891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -1893,7 +1920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1922,7 +1949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1951,7 +1978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1980,7 +2007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2009,7 +2036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -2038,7 +2065,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2067,7 +2094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2113,17 +2140,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2179,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2181,7 +2208,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2218,18 +2245,18 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2246,7 +2273,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2263,7 +2290,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2280,7 +2307,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2297,7 +2324,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2314,7 +2341,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2331,7 +2358,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2348,7 +2375,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2365,7 +2392,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2382,7 +2409,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2399,7 +2426,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2416,7 +2443,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2433,7 +2460,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2450,7 +2477,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2464,7 +2491,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2478,7 +2505,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2492,7 +2519,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2506,7 +2533,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2520,7 +2547,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2534,7 +2561,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2548,7 +2575,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2562,7 +2589,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2576,7 +2603,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2590,7 +2617,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2604,7 +2631,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2618,7 +2645,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2641,22 +2668,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABC4F1-E3E2-CE4D-BF77-D99DAF76AC27}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>236</v>
       </c>
@@ -2679,7 +2706,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>188</v>
       </c>
@@ -2699,7 +2726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>188</v>
       </c>
@@ -2719,10 +2746,10 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -2742,10 +2769,10 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -2765,10 +2792,10 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -2788,10 +2815,10 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -2811,10 +2838,10 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2834,10 +2861,10 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>188</v>
       </c>
@@ -2857,10 +2884,10 @@
         <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -2880,10 +2907,10 @@
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>188</v>
       </c>
@@ -2903,7 +2930,7 @@
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>